<commit_message>
BangChu long datatype, stringFomatter is not recommended, Speech Recognition 50%
</commit_message>
<xml_diff>
--- a/TestFiles/NumberInTextTest.xlsx
+++ b/TestFiles/NumberInTextTest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GR2\MyExcelAddin\TestFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A62E45B-D922-48F6-BE4D-C58EB5548B55}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FEB0EC6-D970-46F7-A797-E26F3F8A0832}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{0C2B33B1-6452-4974-8B12-5857E33D7479}"/>
+    <workbookView xWindow="3360" yWindow="2100" windowWidth="17280" windowHeight="9984" xr2:uid="{0C2B33B1-6452-4974-8B12-5857E33D7479}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -405,13 +405,13 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B32" sqref="B32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.19921875" customWidth="1"/>
-    <col min="2" max="2" width="84.59765625" customWidth="1"/>
+    <col min="2" max="2" width="136" customWidth="1"/>
     <col min="3" max="3" width="79.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -594,13 +594,13 @@
       <c r="A17">
         <v>2147483648</v>
       </c>
-      <c r="B17" t="e" cm="1">
+      <c r="B17" t="str" cm="1">
         <f t="array" ref="B17">_xll.InText(A17)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C17" t="e" cm="1">
+        <v>Two billion, one hundred forty-seven million, four hundred eighty-three thousand, six hundred forty-eight</v>
+      </c>
+      <c r="C17" t="str" cm="1">
         <f t="array" ref="C17">_xll.BangChu(A17)</f>
-        <v>#VALUE!</v>
+        <v>Hai tỷ, một trăm bốn mươi bẩy triệu, bốn trăm tám mươi ba nghìn, sáu trăm bốn mươi tám</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -630,78 +630,78 @@
       <c r="A20">
         <v>12345678912</v>
       </c>
-      <c r="B20" t="e" cm="1">
+      <c r="B20" t="str" cm="1">
         <f t="array" ref="B20">_xll.InText(A20)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C20" t="e" cm="1">
+        <v>Twelve billion, three hundred forty-five million, six hundred seventy-eight thousand, nine hundred twelve</v>
+      </c>
+      <c r="C20" t="str" cm="1">
         <f t="array" ref="C20">_xll.BangChu(A20)</f>
-        <v>#VALUE!</v>
+        <v>Mười hai tỷ, ba trăm bốn mươi lăm triệu, sáu trăm bẩy mươi tám nghìn, chín trăm mười hai</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>10000000000</v>
       </c>
-      <c r="B21" t="e" cm="1">
+      <c r="B21" t="str" cm="1">
         <f t="array" ref="B21">_xll.InText(A21)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C21" t="e" cm="1">
+        <v>Ten billion</v>
+      </c>
+      <c r="C21" t="str" cm="1">
         <f t="array" ref="C21">_xll.BangChu(A21)</f>
-        <v>#VALUE!</v>
+        <v>Mười tỷ</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>9999999999</v>
       </c>
-      <c r="B22" t="e" cm="1">
+      <c r="B22" t="str" cm="1">
         <f t="array" ref="B22">_xll.InText(A22)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C22" t="e" cm="1">
+        <v>Nine billion, nine hundred ninety-nine million, nine hundred ninety-nine thousand, nine hundred ninety-nine</v>
+      </c>
+      <c r="C22" t="str" cm="1">
         <f t="array" ref="C22">_xll.BangChu(A22)</f>
-        <v>#VALUE!</v>
+        <v>Chín tỷ, chín trăm chín mươi chín triệu, chín trăm chín mươi chín nghìn, chín trăm chín mươi chín</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>123456789123</v>
       </c>
-      <c r="B23" t="e" cm="1">
+      <c r="B23" t="str" cm="1">
         <f t="array" ref="B23">_xll.InText(A23)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C23" t="e" cm="1">
+        <v>One hundred twenty-three billion, four hundred fifty-six million, seven hundred eighty-nine thousand, one hundred twenty-three</v>
+      </c>
+      <c r="C23" t="str" cm="1">
         <f t="array" ref="C23">_xll.BangChu(A23)</f>
-        <v>#VALUE!</v>
+        <v>Một trăm hai mươi ba tỷ, bốn trăm năm mươi sáu triệu, bẩy trăm tám mươi chín nghìn, một trăm hai mươi ba</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>123456789123456</v>
       </c>
-      <c r="B24" t="e" cm="1">
+      <c r="B24" t="str" cm="1">
         <f t="array" ref="B24">_xll.InText(A24)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C24" t="e" cm="1">
+        <v>One hundred twenty-threetrillion, four hundred fifty-six billion, seven hundred eighty-nine million, one hundred twenty-three thousand, four hundred fifty-six</v>
+      </c>
+      <c r="C24" t="str" cm="1">
         <f t="array" ref="C24">_xll.BangChu(A24)</f>
-        <v>#VALUE!</v>
+        <v>Một trăm hai mươi ba nghìn tỷ, bốn trăm năm mươi sáu tỷ, bẩy trăm tám mươi chín triệu, một trăm hai mươi ba nghìn, bốn trăm năm mươi sáu</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>1234567891234560</v>
       </c>
-      <c r="B25" t="e" cm="1">
+      <c r="B25" t="str" cm="1">
         <f t="array" ref="B25">_xll.InText(A25)</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C25" t="e" cm="1">
+        <v>One quadrillion, two hundred thirty-fourtrillion, five hundred sixty-seven billion, eight hundred ninety-one million, two hundred thirty-four thousand, five hundred sixty-zero</v>
+      </c>
+      <c r="C25" t="str" cm="1">
         <f t="array" ref="C25">_xll.BangChu(A25)</f>
-        <v>#VALUE!</v>
+        <v>Một triệu tỷ, hai trăm ba mươi bốn nghìn tỷ, năm trăm sáu mươi bẩy tỷ, tám trăm chín mươi mốt triệu, hai trăm ba mươi bốn nghìn, năm trăm sáu mươi</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>